<commit_message>
Casos de entrenamiento actualizados
</commit_message>
<xml_diff>
--- a/Casos_de_entrenamiento.xlsx
+++ b/Casos_de_entrenamiento.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="17">
   <si>
     <t>Genero</t>
   </si>
@@ -44,6 +44,27 @@
   </si>
   <si>
     <t>CABA</t>
+  </si>
+  <si>
+    <t>GBA</t>
+  </si>
+  <si>
+    <t>Cordoba</t>
+  </si>
+  <si>
+    <t>Entre Rios</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>Neuquen</t>
+  </si>
+  <si>
+    <t>Secundario</t>
+  </si>
+  <si>
+    <t>Terciario</t>
   </si>
 </sst>
 </file>
@@ -385,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +417,7 @@
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -423,13 +445,13 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -443,19 +465,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>110000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -463,19 +485,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4">
-        <v>120000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -483,19 +505,19 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5">
-        <v>100000</v>
+        <v>38000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -503,19 +525,19 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6">
-        <v>110000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -523,47 +545,47 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7">
-        <v>120000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8">
-        <v>20000</v>
+        <v>43447</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -575,7 +597,847 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>10000</v>
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>50600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>59989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>27854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>29921</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>56250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>44600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>56320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42">
+        <v>215000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>63100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <v>32000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>